<commit_message>
Update SE1606_SWP391_Online Shop_Weekly Report_W7.xlsx
</commit_message>
<xml_diff>
--- a/Documents/SE1606_SWP391_Online Shop_Weekly Report_W7.xlsx
+++ b/Documents/SE1606_SWP391_Online Shop_Weekly Report_W7.xlsx
@@ -2061,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
-        <v>44724</v>
+        <v>44732</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>107</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
-        <v>44725</v>
+        <v>44733</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>110</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
-        <v>44725</v>
+        <v>44733</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>111</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
-        <v>44727</v>
+        <v>44734</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>73</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>44728</v>
+        <v>44736</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>113</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>44729</v>
+        <v>44737</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>115</v>

</xml_diff>